<commit_message>
fixed wrong pinout for diplom and added dmx pinout
</commit_message>
<xml_diff>
--- a/diplom/pinout.xlsx
+++ b/diplom/pinout.xlsx
@@ -19,17 +19,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
   <si>
     <t>ESP32</t>
   </si>
   <si>
-    <t>GPIO_16</t>
-  </si>
-  <si>
-    <t>GPIO_17</t>
-  </si>
-  <si>
     <t>TX</t>
   </si>
   <si>
@@ -64,6 +58,60 @@
   </si>
   <si>
     <t>AUDIO JACK 2</t>
+  </si>
+  <si>
+    <t>esp32</t>
+  </si>
+  <si>
+    <t>GPIO</t>
+  </si>
+  <si>
+    <t>INFO</t>
+  </si>
+  <si>
+    <t>GPIO16</t>
+  </si>
+  <si>
+    <t>GPIO17</t>
+  </si>
+  <si>
+    <t>NOT RECOMMENDED DUE TO INTERNAL FLASH</t>
+  </si>
+  <si>
+    <t>GPIO_18</t>
+  </si>
+  <si>
+    <t>GPIO_19</t>
+  </si>
+  <si>
+    <t>GPIO_22</t>
+  </si>
+  <si>
+    <t>GPIO_23</t>
+  </si>
+  <si>
+    <t>TX_1</t>
+  </si>
+  <si>
+    <t>RX_1</t>
+  </si>
+  <si>
+    <t>TX_2</t>
+  </si>
+  <si>
+    <t>RX_2</t>
+  </si>
+  <si>
+    <t>DMX</t>
+  </si>
+  <si>
+    <t>GPIO_21</t>
+  </si>
+  <si>
+    <t>RTS</t>
+  </si>
+  <si>
+    <t>GPIO_RTS</t>
   </si>
 </sst>
 </file>
@@ -87,7 +135,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -110,31 +158,17 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -421,96 +455,183 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="L2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="L3" t="s">
+        <v>16</v>
+      </c>
+      <c r="M3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="L4" t="s">
+        <v>17</v>
+      </c>
+      <c r="M4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="5"/>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="5"/>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C6" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C7" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="5"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C8" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C9" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="6"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C10" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>